<commit_message>
Initial Raul Devo push
</commit_message>
<xml_diff>
--- a/Data/Jen Data/Raw data - IWW Monitoring Project - 14th February 2020.xlsx
+++ b/Data/Jen Data/Raw data - IWW Monitoring Project - 14th February 2020.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\injg1\Objcache\Objects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Nextcloud\Github\HiDef\SNH_Moray_Firth\data\Jen Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CECA8792-642D-410D-B363-BBEB0A52123B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="3870" activeTab="1"/>
+    <workbookView xWindow="30315" yWindow="945" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="6" r:id="rId1"/>
@@ -19,24 +20,32 @@
     <sheet name="Rough totals for Volunteers" sheetId="10" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Raw Data'!$A$1:$AC$631</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Raw Data'!$A$1:$AC$640</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Jen Graham</author>
   </authors>
   <commentList>
-    <comment ref="M135" authorId="0" shapeId="0">
+    <comment ref="M135" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -60,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X331" authorId="0" shapeId="0">
+    <comment ref="X331" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -85,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T404" authorId="0" shapeId="0">
+    <comment ref="T404" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -109,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M529" authorId="0" shapeId="0">
+    <comment ref="M529" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -117,7 +126,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Jen Graham:</t>
         </r>
@@ -126,7 +135,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Jen has emailed volunteer - no response
@@ -134,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q554" authorId="0" shapeId="0">
+    <comment ref="Q554" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -142,7 +151,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Jen Graham:</t>
         </r>
@@ -151,7 +160,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Estimate by Jen using description of degrees (in comments) 
@@ -164,12 +173,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Jen Graham</author>
   </authors>
   <commentList>
-    <comment ref="C83" authorId="0" shapeId="0">
+    <comment ref="C83" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -199,7 +208,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7561" uniqueCount="1286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7669" uniqueCount="1303">
   <si>
     <t>Sector (StationName)</t>
   </si>
@@ -4057,17 +4066,68 @@
   </si>
   <si>
     <t>Potential double count with large scoter flock at Golsipe - ID code: 2458916.6.17</t>
+  </si>
+  <si>
+    <t>2458916.I/B5.1</t>
+  </si>
+  <si>
+    <t>Leica APO- Televid 82</t>
+  </si>
+  <si>
+    <t>Kittiwake</t>
+  </si>
+  <si>
+    <t>2 CY Flying</t>
+  </si>
+  <si>
+    <t>2458916.I/B5.2</t>
+  </si>
+  <si>
+    <t>2458916.I/B5.3</t>
+  </si>
+  <si>
+    <t>2458916.I/B5.4</t>
+  </si>
+  <si>
+    <t>2458916.I/B7.1</t>
+  </si>
+  <si>
+    <t>4 male, 3 female</t>
+  </si>
+  <si>
+    <t>I/B2</t>
+  </si>
+  <si>
+    <t>2458916.I/B2.1</t>
+  </si>
+  <si>
+    <t>FE / RW</t>
+  </si>
+  <si>
+    <t>2458916.I/B2.2</t>
+  </si>
+  <si>
+    <t>Black-headed gull</t>
+  </si>
+  <si>
+    <t>NH739578</t>
+  </si>
+  <si>
+    <t>2458916.34.1</t>
+  </si>
+  <si>
+    <t>2458916.34.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4095,19 +4155,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4247,7 +4294,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -4275,7 +4322,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -4288,7 +4335,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -4311,10 +4358,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -4330,28 +4377,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4387,7 +4434,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -4675,8 +4728,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1">
     <tabColor theme="8"/>
   </sheetPr>
   <dimension ref="A3:U19"/>
@@ -4768,7 +4821,7 @@
       </c>
     </row>
     <row r="19" spans="1:1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="58" t="s">
         <v>1283</v>
       </c>
     </row>
@@ -4780,13 +4833,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC631"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:AC640"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="63" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A622" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="S87" sqref="S87"/>
+      <selection pane="bottomLeft" activeCell="A632" sqref="A632:XFD640"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4798,9 +4852,8 @@
     <col min="5" max="5" width="15.7109375" style="16" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" style="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26" style="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.85546875" style="25" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.7109375" style="25" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.7109375" style="25" customWidth="1"/>
     <col min="13" max="13" width="30.42578125" style="2" customWidth="1"/>
@@ -12491,10 +12544,10 @@
       <c r="H114" s="22">
         <v>43849</v>
       </c>
-      <c r="I114" s="61">
+      <c r="I114" s="59">
         <v>0.45833333333333331</v>
       </c>
-      <c r="J114" s="61">
+      <c r="J114" s="59">
         <v>0.54166666666666663</v>
       </c>
       <c r="M114" s="2" t="s">
@@ -12559,10 +12612,10 @@
       <c r="H115" s="22">
         <v>43849</v>
       </c>
-      <c r="I115" s="61">
+      <c r="I115" s="59">
         <v>0.45833333333333331</v>
       </c>
-      <c r="J115" s="61">
+      <c r="J115" s="59">
         <v>0.54166666666666663</v>
       </c>
       <c r="M115" s="2" t="s">
@@ -12627,10 +12680,10 @@
       <c r="H116" s="22">
         <v>43849</v>
       </c>
-      <c r="I116" s="61">
+      <c r="I116" s="59">
         <v>0.45833333333333331</v>
       </c>
-      <c r="J116" s="61">
+      <c r="J116" s="59">
         <v>0.54166666666666663</v>
       </c>
       <c r="M116" s="2" t="s">
@@ -12695,10 +12748,10 @@
       <c r="H117" s="22">
         <v>43849</v>
       </c>
-      <c r="I117" s="61">
+      <c r="I117" s="59">
         <v>0.45833333333333331</v>
       </c>
-      <c r="J117" s="61">
+      <c r="J117" s="59">
         <v>0.54166666666666663</v>
       </c>
       <c r="M117" s="2" t="s">
@@ -12763,10 +12816,10 @@
       <c r="H118" s="22">
         <v>43849</v>
       </c>
-      <c r="I118" s="61">
+      <c r="I118" s="59">
         <v>0.45833333333333331</v>
       </c>
-      <c r="J118" s="61">
+      <c r="J118" s="59">
         <v>0.54166666666666663</v>
       </c>
       <c r="M118" s="2" t="s">
@@ -12831,10 +12884,10 @@
       <c r="H119" s="22">
         <v>43849</v>
       </c>
-      <c r="I119" s="61">
+      <c r="I119" s="59">
         <v>0.45833333333333331</v>
       </c>
-      <c r="J119" s="61">
+      <c r="J119" s="59">
         <v>0.54166666666666663</v>
       </c>
       <c r="M119" s="2" t="s">
@@ -35435,7 +35488,7 @@
         <v>290</v>
       </c>
       <c r="D453" s="35">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E453" s="16" t="s">
         <v>842</v>
@@ -35506,7 +35559,7 @@
         <v>290</v>
       </c>
       <c r="D454" s="35">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E454" s="16" t="s">
         <v>843</v>
@@ -35577,7 +35630,7 @@
         <v>290</v>
       </c>
       <c r="D455" s="35">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E455" s="16" t="s">
         <v>844</v>
@@ -35648,7 +35701,7 @@
         <v>290</v>
       </c>
       <c r="D456" s="35">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E456" s="16" t="s">
         <v>845</v>
@@ -47418,10 +47471,598 @@
         <v>1198</v>
       </c>
     </row>
+    <row r="632" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A632" s="3">
+        <v>2</v>
+      </c>
+      <c r="B632" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C632" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D632" s="35" t="s">
+        <v>710</v>
+      </c>
+      <c r="E632" s="16" t="s">
+        <v>1286</v>
+      </c>
+      <c r="F632" s="7" t="s">
+        <v>1223</v>
+      </c>
+      <c r="G632" s="2" t="s">
+        <v>1131</v>
+      </c>
+      <c r="H632" s="22">
+        <v>43898</v>
+      </c>
+      <c r="I632" s="25">
+        <v>0.39861111111111108</v>
+      </c>
+      <c r="J632" s="25">
+        <v>0.42083333333333334</v>
+      </c>
+      <c r="M632" s="2" t="s">
+        <v>1287</v>
+      </c>
+      <c r="N632" s="7">
+        <v>3</v>
+      </c>
+      <c r="O632" s="7">
+        <v>4</v>
+      </c>
+      <c r="P632">
+        <v>7</v>
+      </c>
+      <c r="Q632" s="28">
+        <v>0</v>
+      </c>
+      <c r="R632" t="s">
+        <v>143</v>
+      </c>
+      <c r="S632" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T632" s="3">
+        <v>2</v>
+      </c>
+      <c r="U632" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W632" t="s">
+        <v>128</v>
+      </c>
+      <c r="X632" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="633" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A633" s="3">
+        <v>2</v>
+      </c>
+      <c r="B633" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C633" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D633" s="35" t="s">
+        <v>710</v>
+      </c>
+      <c r="E633" s="16" t="s">
+        <v>1290</v>
+      </c>
+      <c r="F633" s="7" t="s">
+        <v>1223</v>
+      </c>
+      <c r="G633" s="2" t="s">
+        <v>1131</v>
+      </c>
+      <c r="H633" s="22">
+        <v>43898</v>
+      </c>
+      <c r="I633" s="25">
+        <v>0.39861111111111108</v>
+      </c>
+      <c r="J633" s="25">
+        <v>0.42083333333333334</v>
+      </c>
+      <c r="M633" s="2" t="s">
+        <v>1287</v>
+      </c>
+      <c r="N633" s="7">
+        <v>3</v>
+      </c>
+      <c r="O633" s="7">
+        <v>4</v>
+      </c>
+      <c r="P633">
+        <v>7</v>
+      </c>
+      <c r="Q633" s="28">
+        <v>0</v>
+      </c>
+      <c r="R633" t="s">
+        <v>143</v>
+      </c>
+      <c r="S633" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="T633" s="3">
+        <v>2</v>
+      </c>
+      <c r="U633" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W633">
+        <v>1000</v>
+      </c>
+      <c r="X633" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="634" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A634" s="3">
+        <v>2</v>
+      </c>
+      <c r="B634" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C634" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D634" s="35" t="s">
+        <v>710</v>
+      </c>
+      <c r="E634" s="16" t="s">
+        <v>1291</v>
+      </c>
+      <c r="F634" s="7" t="s">
+        <v>1223</v>
+      </c>
+      <c r="G634" s="2" t="s">
+        <v>1131</v>
+      </c>
+      <c r="H634" s="22">
+        <v>43898</v>
+      </c>
+      <c r="I634" s="25">
+        <v>0.39861111111111108</v>
+      </c>
+      <c r="J634" s="25">
+        <v>0.42083333333333334</v>
+      </c>
+      <c r="M634" s="2" t="s">
+        <v>1287</v>
+      </c>
+      <c r="N634" s="7">
+        <v>3</v>
+      </c>
+      <c r="O634" s="7">
+        <v>4</v>
+      </c>
+      <c r="P634">
+        <v>7</v>
+      </c>
+      <c r="Q634" s="28">
+        <v>0</v>
+      </c>
+      <c r="R634" t="s">
+        <v>143</v>
+      </c>
+      <c r="S634" s="2" t="s">
+        <v>1288</v>
+      </c>
+      <c r="T634" s="3">
+        <v>1</v>
+      </c>
+      <c r="W634" t="s">
+        <v>52</v>
+      </c>
+      <c r="X634" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y634" s="2" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="635" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A635" s="3">
+        <v>2</v>
+      </c>
+      <c r="B635" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C635" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D635" s="35" t="s">
+        <v>710</v>
+      </c>
+      <c r="E635" s="16" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F635" s="7" t="s">
+        <v>1223</v>
+      </c>
+      <c r="G635" s="2" t="s">
+        <v>1131</v>
+      </c>
+      <c r="H635" s="22">
+        <v>43898</v>
+      </c>
+      <c r="I635" s="25">
+        <v>0.39861111111111108</v>
+      </c>
+      <c r="J635" s="25">
+        <v>0.42083333333333334</v>
+      </c>
+      <c r="M635" s="2" t="s">
+        <v>1287</v>
+      </c>
+      <c r="N635" s="7">
+        <v>3</v>
+      </c>
+      <c r="O635" s="7">
+        <v>4</v>
+      </c>
+      <c r="P635">
+        <v>7</v>
+      </c>
+      <c r="Q635" s="28">
+        <v>0</v>
+      </c>
+      <c r="R635" t="s">
+        <v>143</v>
+      </c>
+      <c r="S635" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="T635" s="3">
+        <v>2</v>
+      </c>
+      <c r="U635" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="W635" t="s">
+        <v>128</v>
+      </c>
+      <c r="X635" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="636" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A636" s="3">
+        <v>2</v>
+      </c>
+      <c r="B636" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C636" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D636" s="35" t="s">
+        <v>709</v>
+      </c>
+      <c r="E636" s="16" t="s">
+        <v>1293</v>
+      </c>
+      <c r="F636" s="7" t="s">
+        <v>1222</v>
+      </c>
+      <c r="G636" s="2" t="s">
+        <v>1131</v>
+      </c>
+      <c r="H636" s="22">
+        <v>43898</v>
+      </c>
+      <c r="I636" s="25">
+        <v>0.43472222222222223</v>
+      </c>
+      <c r="J636" s="25">
+        <v>0.4465277777777778</v>
+      </c>
+      <c r="M636" s="2" t="s">
+        <v>1287</v>
+      </c>
+      <c r="N636" s="7">
+        <v>4</v>
+      </c>
+      <c r="O636" s="7">
+        <v>4</v>
+      </c>
+      <c r="P636">
+        <v>5</v>
+      </c>
+      <c r="Q636" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="R636" t="s">
+        <v>143</v>
+      </c>
+      <c r="S636" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="T636" s="3">
+        <v>7</v>
+      </c>
+      <c r="U636" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="W636" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y636" s="2" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="637" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A637" s="3">
+        <v>2</v>
+      </c>
+      <c r="B637" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C637" s="2" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D637" s="35" t="s">
+        <v>1295</v>
+      </c>
+      <c r="E637" s="16" t="s">
+        <v>1296</v>
+      </c>
+      <c r="F637" s="7" t="s">
+        <v>1130</v>
+      </c>
+      <c r="G637" s="2" t="s">
+        <v>1131</v>
+      </c>
+      <c r="H637" s="22">
+        <v>43898</v>
+      </c>
+      <c r="I637" s="25">
+        <v>0.46736111111111112</v>
+      </c>
+      <c r="J637" s="25">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="M637" s="2" t="s">
+        <v>1287</v>
+      </c>
+      <c r="N637" s="7">
+        <v>4</v>
+      </c>
+      <c r="O637" s="7">
+        <v>4</v>
+      </c>
+      <c r="P637">
+        <v>7</v>
+      </c>
+      <c r="Q637" s="28">
+        <v>0.05</v>
+      </c>
+      <c r="R637" t="s">
+        <v>143</v>
+      </c>
+      <c r="S637" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T637" s="3">
+        <v>1</v>
+      </c>
+      <c r="U637" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W637" t="s">
+        <v>52</v>
+      </c>
+      <c r="X637" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="638" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A638" s="3">
+        <v>2</v>
+      </c>
+      <c r="B638" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C638" s="2" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D638" s="35" t="s">
+        <v>1295</v>
+      </c>
+      <c r="E638" s="16" t="s">
+        <v>1298</v>
+      </c>
+      <c r="F638" s="7" t="s">
+        <v>1130</v>
+      </c>
+      <c r="G638" s="2" t="s">
+        <v>1131</v>
+      </c>
+      <c r="H638" s="22">
+        <v>43898</v>
+      </c>
+      <c r="I638" s="25">
+        <v>0.46736111111111112</v>
+      </c>
+      <c r="J638" s="25">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="M638" s="2" t="s">
+        <v>1287</v>
+      </c>
+      <c r="N638" s="7">
+        <v>4</v>
+      </c>
+      <c r="O638" s="7">
+        <v>4</v>
+      </c>
+      <c r="P638">
+        <v>7</v>
+      </c>
+      <c r="Q638" s="28">
+        <v>0.05</v>
+      </c>
+      <c r="R638" t="s">
+        <v>143</v>
+      </c>
+      <c r="S638" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="T638" s="3">
+        <v>4</v>
+      </c>
+      <c r="U638" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="W638" t="s">
+        <v>128</v>
+      </c>
+      <c r="X638" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y638" s="2" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="639" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A639" s="3">
+        <v>2</v>
+      </c>
+      <c r="B639" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C639" s="2" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D639" s="35">
+        <v>34</v>
+      </c>
+      <c r="E639" s="16" t="s">
+        <v>1301</v>
+      </c>
+      <c r="F639" s="7" t="s">
+        <v>1300</v>
+      </c>
+      <c r="G639" s="2" t="s">
+        <v>1131</v>
+      </c>
+      <c r="H639" s="22">
+        <v>43898</v>
+      </c>
+      <c r="I639" s="25">
+        <v>0.51736111111111105</v>
+      </c>
+      <c r="J639" s="25">
+        <v>0.53125</v>
+      </c>
+      <c r="M639" s="2" t="s">
+        <v>1287</v>
+      </c>
+      <c r="N639" s="7">
+        <v>2</v>
+      </c>
+      <c r="O639" s="7">
+        <v>4</v>
+      </c>
+      <c r="P639">
+        <v>6</v>
+      </c>
+      <c r="Q639" s="28">
+        <v>0</v>
+      </c>
+      <c r="R639" t="s">
+        <v>143</v>
+      </c>
+      <c r="S639" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="T639" s="3">
+        <v>78</v>
+      </c>
+      <c r="U639" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="W639" t="s">
+        <v>52</v>
+      </c>
+      <c r="X639" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="640" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A640" s="3">
+        <v>2</v>
+      </c>
+      <c r="B640" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C640" s="2" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D640" s="35">
+        <v>34</v>
+      </c>
+      <c r="E640" s="16" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F640" s="7" t="s">
+        <v>1300</v>
+      </c>
+      <c r="G640" s="2" t="s">
+        <v>1131</v>
+      </c>
+      <c r="H640" s="22">
+        <v>43898</v>
+      </c>
+      <c r="I640" s="25">
+        <v>0.51736111111111105</v>
+      </c>
+      <c r="J640" s="25">
+        <v>0.53125</v>
+      </c>
+      <c r="M640" s="2" t="s">
+        <v>1287</v>
+      </c>
+      <c r="N640" s="7">
+        <v>2</v>
+      </c>
+      <c r="O640" s="7">
+        <v>4</v>
+      </c>
+      <c r="P640">
+        <v>6</v>
+      </c>
+      <c r="Q640" s="28">
+        <v>0</v>
+      </c>
+      <c r="R640" t="s">
+        <v>143</v>
+      </c>
+      <c r="S640" s="2" t="s">
+        <v>1299</v>
+      </c>
+      <c r="T640" s="3">
+        <v>1</v>
+      </c>
+      <c r="U640" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="W640" t="s">
+        <v>52</v>
+      </c>
+      <c r="X640" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AC631"/>
+  <autoFilter ref="A1:AC640" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <dataValidations count="1">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>1</formula1>
       <formula2>2</formula2>
     </dataValidation>
@@ -47432,25 +48073,25 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>'Data Validation'!$C$2:$C$6</xm:f>
           </x14:formula1>
           <xm:sqref>V400:V401</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>'Data Validation'!$B$2:$B$12</xm:f>
           </x14:formula1>
           <xm:sqref>B1:B1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>'Data Validation'!$A:$A</xm:f>
           </x14:formula1>
           <xm:sqref>S1:S1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
             <xm:f>'Data Validation'!$C:$C</xm:f>
           </x14:formula1>
@@ -47463,7 +48104,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:CH92"/>
   <sheetViews>
     <sheetView zoomScale="82" workbookViewId="0">
@@ -48001,30 +48643,30 @@
       <c r="CH4" s="44"/>
     </row>
     <row r="7" spans="2:86" x14ac:dyDescent="0.25">
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="60" t="s">
         <v>1258</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="59"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="61"/>
       <c r="F7" s="49"/>
     </row>
     <row r="8" spans="2:86" x14ac:dyDescent="0.25">
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="60" t="s">
         <v>1259</v>
       </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="59"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="61"/>
       <c r="F8" s="50"/>
     </row>
     <row r="9" spans="2:86" x14ac:dyDescent="0.25">
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="60" t="s">
         <v>1260</v>
       </c>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="59"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="61"/>
       <c r="F9" s="52"/>
     </row>
     <row r="10" spans="2:86" x14ac:dyDescent="0.25">
@@ -48290,11 +48932,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48574,13 +49217,24 @@
         <v>1240</v>
       </c>
     </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>1299</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -48594,14 +49248,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>1280</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="D1" s="58" t="s">
+      <c r="B1" s="60"/>
+      <c r="D1" s="60" t="s">
         <v>1279</v>
       </c>
-      <c r="E1" s="58"/>
+      <c r="E1" s="60"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -49069,7 +49723,7 @@
 </worksheet>
 </file>
 
-<file path=customXML/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://www.objective.com/ecm/document/metadata/71FFD1B571BE2883E0537D20C80A46C7" version="1.0.0">
   <systemFields>
     <field name="Objective-Id">
@@ -49094,7 +49748,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-04-28T15:04:22Z</value>
+      <value order="0">2020-05-19T08:53:41Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Jen Graham</value>
@@ -49109,13 +49763,13 @@
       <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA5691661</value>
+      <value order="0">vA5715558</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">0.21</value>
+      <value order="0">0.23</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">21</value>
+      <value order="0">23</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>
@@ -49173,7 +49827,7 @@
 </metadata>
 </file>
 
-<file path=customXML/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5745109E-2DDF-40CB-AC2B-FF9B10C90820}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.objective.com/ecm/document/metadata/71FFD1B571BE2883E0537D20C80A46C7"/>

</xml_diff>